<commit_message>
added image of gantt chart to org doc
</commit_message>
<xml_diff>
--- a/docs/TopperNav Gantt Chart.xlsx
+++ b/docs/TopperNav Gantt Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/014b0dfa241f4418/Desktop/TopperNav/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="11_3C4179B01545E19DD6C385890107473B0B440F85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31C58EAF-26AA-4A5B-A8DB-15172786A36E}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="11_3C4179B01545E19DD6C385890107473B0B440F85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{103C8527-B2C6-4E2A-B497-FA330A4EA448}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3348" yWindow="3348" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>TopperNav</t>
   </si>
@@ -161,9 +161,6 @@
     <t xml:space="preserve">Team Creation </t>
   </si>
   <si>
-    <t>Documentation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Presentation </t>
   </si>
   <si>
@@ -174,6 +171,24 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Kayden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gantt Chart </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aaron </t>
+  </si>
+  <si>
+    <t>Orginzational Doc</t>
+  </si>
+  <si>
+    <t>Techical Doc</t>
+  </si>
+  <si>
+    <t>Ryerson</t>
   </si>
 </sst>
 </file>
@@ -790,7 +805,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1121,6 +1136,21 @@
     </xf>
     <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1724,10 +1754,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL36"/>
+  <dimension ref="A1:BL38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2455,7 +2485,7 @@
       <c r="F8" s="44"/>
       <c r="G8" s="17"/>
       <c r="H8" s="5" t="str">
-        <f t="shared" ref="H8:H33" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H35" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="45"/>
@@ -2518,13 +2548,13 @@
     <row r="9" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="47" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="49">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="50">
         <f>J5</f>
@@ -2599,25 +2629,24 @@
     <row r="10" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="53">
-        <v>0.8</v>
-      </c>
-      <c r="E10" s="54">
-        <f>S5</f>
-        <v>45897</v>
-      </c>
-      <c r="F10" s="54">
-        <f>E10+2</f>
-        <v>45899</v>
+        <v>43</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="49">
+        <v>1</v>
+      </c>
+      <c r="E10" s="50">
+        <f>J5</f>
+        <v>45888</v>
+      </c>
+      <c r="F10" s="50">
+        <f>X5</f>
+        <v>45902</v>
       </c>
       <c r="G10" s="17"/>
-      <c r="H10" s="5">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
+      <c r="H10" s="5"/>
       <c r="I10" s="51"/>
       <c r="J10" s="51"/>
       <c r="K10" s="51"/>
@@ -2630,8 +2659,8 @@
       <c r="R10" s="51"/>
       <c r="S10" s="51"/>
       <c r="T10" s="51"/>
-      <c r="U10" s="55"/>
-      <c r="V10" s="55"/>
+      <c r="U10" s="51"/>
+      <c r="V10" s="51"/>
       <c r="W10" s="51"/>
       <c r="X10" s="51"/>
       <c r="Y10" s="51"/>
@@ -2676,28 +2705,28 @@
       <c r="BL10" s="51"/>
     </row>
     <row r="11" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="53">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E11" s="54">
-        <f>J5</f>
-        <v>45888</v>
+        <f>S5</f>
+        <v>45897</v>
       </c>
       <c r="F11" s="54">
-        <f ca="1">TODAY()</f>
-        <v>45897</v>
+        <f>E11+2</f>
+        <v>45899</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="I11" s="51"/>
       <c r="J11" s="51"/>
@@ -2711,8 +2740,8 @@
       <c r="R11" s="51"/>
       <c r="S11" s="51"/>
       <c r="T11" s="51"/>
-      <c r="U11" s="51"/>
-      <c r="V11" s="51"/>
+      <c r="U11" s="55"/>
+      <c r="V11" s="55"/>
       <c r="W11" s="51"/>
       <c r="X11" s="51"/>
       <c r="Y11" s="51"/>
@@ -2762,23 +2791,21 @@
         <v>38</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="53">
-        <v>1</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D12" s="53"/>
       <c r="E12" s="54">
-        <f ca="1">F11</f>
+        <f>J5</f>
+        <v>45888</v>
+      </c>
+      <c r="F12" s="54">
+        <f ca="1">TODAY()</f>
         <v>45897</v>
-      </c>
-      <c r="F12" s="54">
-        <f ca="1">E12+5</f>
-        <v>45902</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I12" s="51"/>
       <c r="J12" s="51"/>
@@ -2796,7 +2823,7 @@
       <c r="V12" s="51"/>
       <c r="W12" s="51"/>
       <c r="X12" s="51"/>
-      <c r="Y12" s="55"/>
+      <c r="Y12" s="51"/>
       <c r="Z12" s="51"/>
       <c r="AA12" s="51"/>
       <c r="AB12" s="51"/>
@@ -2840,24 +2867,26 @@
     <row r="13" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="47" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="53"/>
+        <v>39</v>
+      </c>
+      <c r="D13" s="53">
+        <v>1</v>
+      </c>
       <c r="E13" s="54">
-        <f>Q1</f>
-        <v>45888</v>
+        <f ca="1">F12</f>
+        <v>45897</v>
       </c>
       <c r="F13" s="54">
-        <f>Q1</f>
-        <v>45888</v>
+        <f ca="1">E13+5</f>
+        <v>45902</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="5">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
       </c>
       <c r="I13" s="51"/>
       <c r="J13" s="51"/>
@@ -2875,7 +2904,7 @@
       <c r="V13" s="51"/>
       <c r="W13" s="51"/>
       <c r="X13" s="51"/>
-      <c r="Y13" s="51"/>
+      <c r="Y13" s="55"/>
       <c r="Z13" s="51"/>
       <c r="AA13" s="51"/>
       <c r="AB13" s="51"/>
@@ -2917,197 +2946,200 @@
       <c r="BL13" s="51"/>
     </row>
     <row r="14" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="56" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="53">
+        <v>1</v>
+      </c>
+      <c r="E14" s="54">
+        <f>Q1</f>
+        <v>45888</v>
+      </c>
+      <c r="F14" s="54">
+        <f>Q1</f>
+        <v>45888</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="5">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="51"/>
+      <c r="AA14" s="51"/>
+      <c r="AB14" s="51"/>
+      <c r="AC14" s="51"/>
+      <c r="AD14" s="51"/>
+      <c r="AE14" s="51"/>
+      <c r="AF14" s="51"/>
+      <c r="AG14" s="51"/>
+      <c r="AH14" s="51"/>
+      <c r="AI14" s="51"/>
+      <c r="AJ14" s="51"/>
+      <c r="AK14" s="51"/>
+      <c r="AL14" s="51"/>
+      <c r="AM14" s="51"/>
+      <c r="AN14" s="51"/>
+      <c r="AO14" s="51"/>
+      <c r="AP14" s="51"/>
+      <c r="AQ14" s="51"/>
+      <c r="AR14" s="51"/>
+      <c r="AS14" s="51"/>
+      <c r="AT14" s="51"/>
+      <c r="AU14" s="51"/>
+      <c r="AV14" s="51"/>
+      <c r="AW14" s="51"/>
+      <c r="AX14" s="51"/>
+      <c r="AY14" s="51"/>
+      <c r="AZ14" s="51"/>
+      <c r="BA14" s="51"/>
+      <c r="BB14" s="51"/>
+      <c r="BC14" s="51"/>
+      <c r="BD14" s="51"/>
+      <c r="BE14" s="51"/>
+      <c r="BF14" s="51"/>
+      <c r="BG14" s="51"/>
+      <c r="BH14" s="51"/>
+      <c r="BI14" s="51"/>
+      <c r="BJ14" s="51"/>
+      <c r="BK14" s="51"/>
+      <c r="BL14" s="51"/>
+    </row>
+    <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="121" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="122" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="123">
+        <v>1</v>
+      </c>
+      <c r="E15" s="124">
+        <f>I5</f>
+        <v>45887</v>
+      </c>
+      <c r="F15" s="124">
+        <f>X5</f>
+        <v>45902</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="125"/>
+      <c r="J15" s="125"/>
+      <c r="K15" s="125"/>
+      <c r="L15" s="125"/>
+      <c r="M15" s="125"/>
+      <c r="N15" s="125"/>
+      <c r="O15" s="125"/>
+      <c r="P15" s="125"/>
+      <c r="Q15" s="125"/>
+      <c r="R15" s="125"/>
+      <c r="S15" s="125"/>
+      <c r="T15" s="125"/>
+      <c r="U15" s="125"/>
+      <c r="V15" s="125"/>
+      <c r="W15" s="125"/>
+      <c r="X15" s="125"/>
+      <c r="Y15" s="125"/>
+      <c r="Z15" s="125"/>
+      <c r="AA15" s="125"/>
+      <c r="AB15" s="125"/>
+      <c r="AC15" s="125"/>
+      <c r="AD15" s="125"/>
+      <c r="AE15" s="125"/>
+      <c r="AF15" s="125"/>
+      <c r="AG15" s="125"/>
+      <c r="AH15" s="125"/>
+      <c r="AI15" s="125"/>
+      <c r="AJ15" s="125"/>
+      <c r="AK15" s="125"/>
+      <c r="AL15" s="125"/>
+      <c r="AM15" s="125"/>
+      <c r="AN15" s="125"/>
+      <c r="AO15" s="125"/>
+      <c r="AP15" s="125"/>
+      <c r="AQ15" s="125"/>
+      <c r="AR15" s="125"/>
+      <c r="AS15" s="125"/>
+      <c r="AT15" s="125"/>
+      <c r="AU15" s="125"/>
+      <c r="AV15" s="125"/>
+      <c r="AW15" s="125"/>
+      <c r="AX15" s="125"/>
+      <c r="AY15" s="125"/>
+      <c r="AZ15" s="125"/>
+      <c r="BA15" s="125"/>
+      <c r="BB15" s="125"/>
+      <c r="BC15" s="125"/>
+      <c r="BD15" s="125"/>
+      <c r="BE15" s="125"/>
+      <c r="BF15" s="125"/>
+      <c r="BG15" s="125"/>
+      <c r="BH15" s="125"/>
+      <c r="BI15" s="125"/>
+      <c r="BJ15" s="125"/>
+      <c r="BK15" s="125"/>
+      <c r="BL15" s="125"/>
+    </row>
+    <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="5" t="str">
+      <c r="C16" s="57"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="5" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="61" t="s">
+    <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63">
+      <c r="C17" s="62"/>
+      <c r="D17" s="63">
         <v>0.5</v>
       </c>
-      <c r="E15" s="64">
-        <f>E13+1</f>
+      <c r="E17" s="64">
+        <f>E14+1</f>
         <v>45889</v>
       </c>
-      <c r="F15" s="64">
-        <f>E15+4</f>
+      <c r="F17" s="64">
+        <f>E17+4</f>
         <v>45893</v>
-      </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="5">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="51"/>
-      <c r="T15" s="51"/>
-      <c r="U15" s="51"/>
-      <c r="V15" s="51"/>
-      <c r="W15" s="51"/>
-      <c r="X15" s="51"/>
-      <c r="Y15" s="51"/>
-      <c r="Z15" s="51"/>
-      <c r="AA15" s="51"/>
-      <c r="AB15" s="51"/>
-      <c r="AC15" s="51"/>
-      <c r="AD15" s="51"/>
-      <c r="AE15" s="51"/>
-      <c r="AF15" s="51"/>
-      <c r="AG15" s="51"/>
-      <c r="AH15" s="51"/>
-      <c r="AI15" s="51"/>
-      <c r="AJ15" s="51"/>
-      <c r="AK15" s="51"/>
-      <c r="AL15" s="51"/>
-      <c r="AM15" s="51"/>
-      <c r="AN15" s="51"/>
-      <c r="AO15" s="51"/>
-      <c r="AP15" s="51"/>
-      <c r="AQ15" s="51"/>
-      <c r="AR15" s="51"/>
-      <c r="AS15" s="51"/>
-      <c r="AT15" s="51"/>
-      <c r="AU15" s="51"/>
-      <c r="AV15" s="51"/>
-      <c r="AW15" s="51"/>
-      <c r="AX15" s="51"/>
-      <c r="AY15" s="51"/>
-      <c r="AZ15" s="51"/>
-      <c r="BA15" s="51"/>
-      <c r="BB15" s="51"/>
-      <c r="BC15" s="51"/>
-      <c r="BD15" s="51"/>
-      <c r="BE15" s="51"/>
-      <c r="BF15" s="51"/>
-      <c r="BG15" s="51"/>
-      <c r="BH15" s="51"/>
-      <c r="BI15" s="51"/>
-      <c r="BJ15" s="51"/>
-      <c r="BK15" s="51"/>
-      <c r="BL15" s="51"/>
-    </row>
-    <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="64">
-        <f>E15+2</f>
-        <v>45891</v>
-      </c>
-      <c r="F16" s="64">
-        <f>E16+5</f>
-        <v>45896</v>
-      </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="5">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="51"/>
-      <c r="S16" s="51"/>
-      <c r="T16" s="51"/>
-      <c r="U16" s="55"/>
-      <c r="V16" s="55"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="51"/>
-      <c r="Y16" s="51"/>
-      <c r="Z16" s="51"/>
-      <c r="AA16" s="51"/>
-      <c r="AB16" s="51"/>
-      <c r="AC16" s="51"/>
-      <c r="AD16" s="51"/>
-      <c r="AE16" s="51"/>
-      <c r="AF16" s="51"/>
-      <c r="AG16" s="51"/>
-      <c r="AH16" s="51"/>
-      <c r="AI16" s="51"/>
-      <c r="AJ16" s="51"/>
-      <c r="AK16" s="51"/>
-      <c r="AL16" s="51"/>
-      <c r="AM16" s="51"/>
-      <c r="AN16" s="51"/>
-      <c r="AO16" s="51"/>
-      <c r="AP16" s="51"/>
-      <c r="AQ16" s="51"/>
-      <c r="AR16" s="51"/>
-      <c r="AS16" s="51"/>
-      <c r="AT16" s="51"/>
-      <c r="AU16" s="51"/>
-      <c r="AV16" s="51"/>
-      <c r="AW16" s="51"/>
-      <c r="AX16" s="51"/>
-      <c r="AY16" s="51"/>
-      <c r="AZ16" s="51"/>
-      <c r="BA16" s="51"/>
-      <c r="BB16" s="51"/>
-      <c r="BC16" s="51"/>
-      <c r="BD16" s="51"/>
-      <c r="BE16" s="51"/>
-      <c r="BF16" s="51"/>
-      <c r="BG16" s="51"/>
-      <c r="BH16" s="51"/>
-      <c r="BI16" s="51"/>
-      <c r="BJ16" s="51"/>
-      <c r="BK16" s="51"/>
-      <c r="BL16" s="51"/>
-    </row>
-    <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="64">
-        <f>F16</f>
-        <v>45896</v>
-      </c>
-      <c r="F17" s="64">
-        <f>E17+3</f>
-        <v>45899</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I17" s="51"/>
       <c r="J17" s="51"/>
@@ -3169,22 +3201,24 @@
     <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="61" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
+      <c r="D18" s="63">
+        <v>0.5</v>
+      </c>
       <c r="E18" s="64">
-        <f>E17</f>
+        <f>E17+2</f>
+        <v>45891</v>
+      </c>
+      <c r="F18" s="64">
+        <f>E18+5</f>
         <v>45896</v>
-      </c>
-      <c r="F18" s="64">
-        <f>E18+2</f>
-        <v>45898</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="5">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I18" s="51"/>
       <c r="J18" s="51"/>
@@ -3198,11 +3232,11 @@
       <c r="R18" s="51"/>
       <c r="S18" s="51"/>
       <c r="T18" s="51"/>
-      <c r="U18" s="51"/>
-      <c r="V18" s="51"/>
+      <c r="U18" s="55"/>
+      <c r="V18" s="55"/>
       <c r="W18" s="51"/>
       <c r="X18" s="51"/>
-      <c r="Y18" s="55"/>
+      <c r="Y18" s="51"/>
       <c r="Z18" s="51"/>
       <c r="AA18" s="51"/>
       <c r="AB18" s="51"/>
@@ -3246,12 +3280,12 @@
     <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="61" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" s="62"/>
       <c r="D19" s="63"/>
       <c r="E19" s="64">
-        <f>E18</f>
+        <f>F18</f>
         <v>45896</v>
       </c>
       <c r="F19" s="64">
@@ -3322,96 +3356,100 @@
     </row>
     <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
-      <c r="B20" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="66"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="69"/>
+      <c r="B20" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="64">
+        <f>E19</f>
+        <v>45896</v>
+      </c>
+      <c r="F20" s="64">
+        <f>E20+2</f>
+        <v>45898</v>
+      </c>
       <c r="G20" s="17"/>
-      <c r="H20" s="5" t="str">
+      <c r="H20" s="5">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I20" s="70"/>
-      <c r="J20" s="70"/>
-      <c r="K20" s="70"/>
-      <c r="L20" s="70"/>
-      <c r="M20" s="70"/>
-      <c r="N20" s="70"/>
-      <c r="O20" s="70"/>
-      <c r="P20" s="70"/>
-      <c r="Q20" s="70"/>
-      <c r="R20" s="70"/>
-      <c r="S20" s="70"/>
-      <c r="T20" s="70"/>
-      <c r="U20" s="70"/>
-      <c r="V20" s="70"/>
-      <c r="W20" s="70"/>
-      <c r="X20" s="70"/>
-      <c r="Y20" s="70"/>
-      <c r="Z20" s="70"/>
-      <c r="AA20" s="70"/>
-      <c r="AB20" s="70"/>
-      <c r="AC20" s="70"/>
-      <c r="AD20" s="70"/>
-      <c r="AE20" s="70"/>
-      <c r="AF20" s="70"/>
-      <c r="AG20" s="70"/>
-      <c r="AH20" s="70"/>
-      <c r="AI20" s="70"/>
-      <c r="AJ20" s="70"/>
-      <c r="AK20" s="70"/>
-      <c r="AL20" s="70"/>
-      <c r="AM20" s="70"/>
-      <c r="AN20" s="70"/>
-      <c r="AO20" s="70"/>
-      <c r="AP20" s="70"/>
-      <c r="AQ20" s="70"/>
-      <c r="AR20" s="70"/>
-      <c r="AS20" s="70"/>
-      <c r="AT20" s="70"/>
-      <c r="AU20" s="70"/>
-      <c r="AV20" s="70"/>
-      <c r="AW20" s="70"/>
-      <c r="AX20" s="70"/>
-      <c r="AY20" s="70"/>
-      <c r="AZ20" s="70"/>
-      <c r="BA20" s="70"/>
-      <c r="BB20" s="70"/>
-      <c r="BC20" s="70"/>
-      <c r="BD20" s="70"/>
-      <c r="BE20" s="70"/>
-      <c r="BF20" s="70"/>
-      <c r="BG20" s="70"/>
-      <c r="BH20" s="70"/>
-      <c r="BI20" s="70"/>
-      <c r="BJ20" s="70"/>
-      <c r="BK20" s="70"/>
-      <c r="BL20" s="70"/>
+        <v>3</v>
+      </c>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
+      <c r="X20" s="51"/>
+      <c r="Y20" s="55"/>
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="51"/>
+      <c r="AB20" s="51"/>
+      <c r="AC20" s="51"/>
+      <c r="AD20" s="51"/>
+      <c r="AE20" s="51"/>
+      <c r="AF20" s="51"/>
+      <c r="AG20" s="51"/>
+      <c r="AH20" s="51"/>
+      <c r="AI20" s="51"/>
+      <c r="AJ20" s="51"/>
+      <c r="AK20" s="51"/>
+      <c r="AL20" s="51"/>
+      <c r="AM20" s="51"/>
+      <c r="AN20" s="51"/>
+      <c r="AO20" s="51"/>
+      <c r="AP20" s="51"/>
+      <c r="AQ20" s="51"/>
+      <c r="AR20" s="51"/>
+      <c r="AS20" s="51"/>
+      <c r="AT20" s="51"/>
+      <c r="AU20" s="51"/>
+      <c r="AV20" s="51"/>
+      <c r="AW20" s="51"/>
+      <c r="AX20" s="51"/>
+      <c r="AY20" s="51"/>
+      <c r="AZ20" s="51"/>
+      <c r="BA20" s="51"/>
+      <c r="BB20" s="51"/>
+      <c r="BC20" s="51"/>
+      <c r="BD20" s="51"/>
+      <c r="BE20" s="51"/>
+      <c r="BF20" s="51"/>
+      <c r="BG20" s="51"/>
+      <c r="BH20" s="51"/>
+      <c r="BI20" s="51"/>
+      <c r="BJ20" s="51"/>
+      <c r="BK20" s="51"/>
+      <c r="BL20" s="51"/>
     </row>
     <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
-      <c r="B21" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="73">
-        <v>0.5</v>
-      </c>
-      <c r="E21" s="74">
-        <f>E9+15</f>
-        <v>45903</v>
-      </c>
-      <c r="F21" s="74">
-        <f>E21+5</f>
-        <v>45908</v>
+      <c r="B21" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="62"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="64">
+        <f>E20</f>
+        <v>45896</v>
+      </c>
+      <c r="F21" s="64">
+        <f>E21+3</f>
+        <v>45899</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I21" s="51"/>
       <c r="J21" s="51"/>
@@ -3472,99 +3510,91 @@
     </row>
     <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
-      <c r="B22" s="71" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="72"/>
-      <c r="D22" s="73">
-        <v>0.6</v>
-      </c>
-      <c r="E22" s="74">
-        <f>F21+1</f>
-        <v>45909</v>
-      </c>
-      <c r="F22" s="74">
-        <f>E22+4</f>
-        <v>45913</v>
-      </c>
+      <c r="B22" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="66"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="69"/>
       <c r="G22" s="17"/>
-      <c r="H22" s="5">
+      <c r="H22" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="51"/>
-      <c r="P22" s="51"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="51"/>
-      <c r="S22" s="51"/>
-      <c r="T22" s="51"/>
-      <c r="U22" s="51"/>
-      <c r="V22" s="51"/>
-      <c r="W22" s="51"/>
-      <c r="X22" s="51"/>
-      <c r="Y22" s="51"/>
-      <c r="Z22" s="51"/>
-      <c r="AA22" s="51"/>
-      <c r="AB22" s="51"/>
-      <c r="AC22" s="51"/>
-      <c r="AD22" s="51"/>
-      <c r="AE22" s="51"/>
-      <c r="AF22" s="51"/>
-      <c r="AG22" s="51"/>
-      <c r="AH22" s="51"/>
-      <c r="AI22" s="51"/>
-      <c r="AJ22" s="51"/>
-      <c r="AK22" s="51"/>
-      <c r="AL22" s="51"/>
-      <c r="AM22" s="51"/>
-      <c r="AN22" s="51"/>
-      <c r="AO22" s="51"/>
-      <c r="AP22" s="51"/>
-      <c r="AQ22" s="51"/>
-      <c r="AR22" s="51"/>
-      <c r="AS22" s="51"/>
-      <c r="AT22" s="51"/>
-      <c r="AU22" s="51"/>
-      <c r="AV22" s="51"/>
-      <c r="AW22" s="51"/>
-      <c r="AX22" s="51"/>
-      <c r="AY22" s="51"/>
-      <c r="AZ22" s="51"/>
-      <c r="BA22" s="51"/>
-      <c r="BB22" s="51"/>
-      <c r="BC22" s="51"/>
-      <c r="BD22" s="51"/>
-      <c r="BE22" s="51"/>
-      <c r="BF22" s="51"/>
-      <c r="BG22" s="51"/>
-      <c r="BH22" s="51"/>
-      <c r="BI22" s="51"/>
-      <c r="BJ22" s="51"/>
-      <c r="BK22" s="51"/>
-      <c r="BL22" s="51"/>
+        <v/>
+      </c>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="70"/>
+      <c r="M22" s="70"/>
+      <c r="N22" s="70"/>
+      <c r="O22" s="70"/>
+      <c r="P22" s="70"/>
+      <c r="Q22" s="70"/>
+      <c r="R22" s="70"/>
+      <c r="S22" s="70"/>
+      <c r="T22" s="70"/>
+      <c r="U22" s="70"/>
+      <c r="V22" s="70"/>
+      <c r="W22" s="70"/>
+      <c r="X22" s="70"/>
+      <c r="Y22" s="70"/>
+      <c r="Z22" s="70"/>
+      <c r="AA22" s="70"/>
+      <c r="AB22" s="70"/>
+      <c r="AC22" s="70"/>
+      <c r="AD22" s="70"/>
+      <c r="AE22" s="70"/>
+      <c r="AF22" s="70"/>
+      <c r="AG22" s="70"/>
+      <c r="AH22" s="70"/>
+      <c r="AI22" s="70"/>
+      <c r="AJ22" s="70"/>
+      <c r="AK22" s="70"/>
+      <c r="AL22" s="70"/>
+      <c r="AM22" s="70"/>
+      <c r="AN22" s="70"/>
+      <c r="AO22" s="70"/>
+      <c r="AP22" s="70"/>
+      <c r="AQ22" s="70"/>
+      <c r="AR22" s="70"/>
+      <c r="AS22" s="70"/>
+      <c r="AT22" s="70"/>
+      <c r="AU22" s="70"/>
+      <c r="AV22" s="70"/>
+      <c r="AW22" s="70"/>
+      <c r="AX22" s="70"/>
+      <c r="AY22" s="70"/>
+      <c r="AZ22" s="70"/>
+      <c r="BA22" s="70"/>
+      <c r="BB22" s="70"/>
+      <c r="BC22" s="70"/>
+      <c r="BD22" s="70"/>
+      <c r="BE22" s="70"/>
+      <c r="BF22" s="70"/>
+      <c r="BG22" s="70"/>
+      <c r="BH22" s="70"/>
+      <c r="BI22" s="70"/>
+      <c r="BJ22" s="70"/>
+      <c r="BK22" s="70"/>
+      <c r="BL22" s="70"/>
     </row>
     <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="71" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C23" s="72"/>
       <c r="D23" s="73">
         <v>0.5</v>
       </c>
       <c r="E23" s="74">
-        <f>E22+5</f>
-        <v>45914</v>
+        <f>E9+15</f>
+        <v>45903</v>
       </c>
       <c r="F23" s="74">
         <f>E23+5</f>
-        <v>45919</v>
+        <v>45908</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="5">
@@ -3631,19 +3661,19 @@
     <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="71" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" s="72"/>
       <c r="D24" s="73">
-        <v>0.25</v>
+        <v>0.6</v>
       </c>
       <c r="E24" s="74">
         <f>F23+1</f>
-        <v>45920</v>
+        <v>45909</v>
       </c>
       <c r="F24" s="74">
         <f>E24+4</f>
-        <v>45924</v>
+        <v>45913</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="5">
@@ -3710,24 +3740,24 @@
     <row r="25" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="71" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C25" s="72"/>
       <c r="D25" s="73">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E25" s="74">
-        <f>E23</f>
+        <f>E24+5</f>
         <v>45914</v>
       </c>
       <c r="F25" s="74">
-        <f>E25+4</f>
-        <v>45918</v>
+        <f>E25+5</f>
+        <v>45919</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I25" s="51"/>
       <c r="J25" s="51"/>
@@ -3788,96 +3818,104 @@
     </row>
     <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
-      <c r="B26" s="75" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="79"/>
+      <c r="B26" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="72"/>
+      <c r="D26" s="73">
+        <v>0.25</v>
+      </c>
+      <c r="E26" s="74">
+        <f>F25+1</f>
+        <v>45920</v>
+      </c>
+      <c r="F26" s="74">
+        <f>E26+4</f>
+        <v>45924</v>
+      </c>
       <c r="G26" s="17"/>
-      <c r="H26" s="5" t="str">
+      <c r="H26" s="5">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="80"/>
-      <c r="L26" s="80"/>
-      <c r="M26" s="80"/>
-      <c r="N26" s="80"/>
-      <c r="O26" s="80"/>
-      <c r="P26" s="80"/>
-      <c r="Q26" s="80"/>
-      <c r="R26" s="80"/>
-      <c r="S26" s="80"/>
-      <c r="T26" s="80"/>
-      <c r="U26" s="80"/>
-      <c r="V26" s="80"/>
-      <c r="W26" s="80"/>
-      <c r="X26" s="80"/>
-      <c r="Y26" s="80"/>
-      <c r="Z26" s="80"/>
-      <c r="AA26" s="80"/>
-      <c r="AB26" s="80"/>
-      <c r="AC26" s="80"/>
-      <c r="AD26" s="80"/>
-      <c r="AE26" s="80"/>
-      <c r="AF26" s="80"/>
-      <c r="AG26" s="80"/>
-      <c r="AH26" s="80"/>
-      <c r="AI26" s="80"/>
-      <c r="AJ26" s="80"/>
-      <c r="AK26" s="80"/>
-      <c r="AL26" s="80"/>
-      <c r="AM26" s="80"/>
-      <c r="AN26" s="80"/>
-      <c r="AO26" s="80"/>
-      <c r="AP26" s="80"/>
-      <c r="AQ26" s="80"/>
-      <c r="AR26" s="80"/>
-      <c r="AS26" s="80"/>
-      <c r="AT26" s="80"/>
-      <c r="AU26" s="80"/>
-      <c r="AV26" s="80"/>
-      <c r="AW26" s="80"/>
-      <c r="AX26" s="80"/>
-      <c r="AY26" s="80"/>
-      <c r="AZ26" s="80"/>
-      <c r="BA26" s="80"/>
-      <c r="BB26" s="80"/>
-      <c r="BC26" s="80"/>
-      <c r="BD26" s="80"/>
-      <c r="BE26" s="80"/>
-      <c r="BF26" s="80"/>
-      <c r="BG26" s="80"/>
-      <c r="BH26" s="80"/>
-      <c r="BI26" s="80"/>
-      <c r="BJ26" s="80"/>
-      <c r="BK26" s="80"/>
-      <c r="BL26" s="80"/>
+        <v>5</v>
+      </c>
+      <c r="I26" s="51"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="51"/>
+      <c r="L26" s="51"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="51"/>
+      <c r="S26" s="51"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="51"/>
+      <c r="X26" s="51"/>
+      <c r="Y26" s="51"/>
+      <c r="Z26" s="51"/>
+      <c r="AA26" s="51"/>
+      <c r="AB26" s="51"/>
+      <c r="AC26" s="51"/>
+      <c r="AD26" s="51"/>
+      <c r="AE26" s="51"/>
+      <c r="AF26" s="51"/>
+      <c r="AG26" s="51"/>
+      <c r="AH26" s="51"/>
+      <c r="AI26" s="51"/>
+      <c r="AJ26" s="51"/>
+      <c r="AK26" s="51"/>
+      <c r="AL26" s="51"/>
+      <c r="AM26" s="51"/>
+      <c r="AN26" s="51"/>
+      <c r="AO26" s="51"/>
+      <c r="AP26" s="51"/>
+      <c r="AQ26" s="51"/>
+      <c r="AR26" s="51"/>
+      <c r="AS26" s="51"/>
+      <c r="AT26" s="51"/>
+      <c r="AU26" s="51"/>
+      <c r="AV26" s="51"/>
+      <c r="AW26" s="51"/>
+      <c r="AX26" s="51"/>
+      <c r="AY26" s="51"/>
+      <c r="AZ26" s="51"/>
+      <c r="BA26" s="51"/>
+      <c r="BB26" s="51"/>
+      <c r="BC26" s="51"/>
+      <c r="BD26" s="51"/>
+      <c r="BE26" s="51"/>
+      <c r="BF26" s="51"/>
+      <c r="BG26" s="51"/>
+      <c r="BH26" s="51"/>
+      <c r="BI26" s="51"/>
+      <c r="BJ26" s="51"/>
+      <c r="BK26" s="51"/>
+      <c r="BL26" s="51"/>
     </row>
     <row r="27" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
-      <c r="B27" s="81" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="82"/>
-      <c r="D27" s="83">
+      <c r="B27" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="72"/>
+      <c r="D27" s="73">
         <v>0.25</v>
       </c>
-      <c r="E27" s="84">
-        <f>E21+2</f>
-        <v>45905</v>
-      </c>
-      <c r="F27" s="84">
-        <f>E27+3</f>
-        <v>45908</v>
+      <c r="E27" s="74">
+        <f>E25</f>
+        <v>45914</v>
+      </c>
+      <c r="F27" s="74">
+        <f>E27+4</f>
+        <v>45918</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I27" s="51"/>
       <c r="J27" s="51"/>
@@ -3938,99 +3976,91 @@
     </row>
     <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
-      <c r="B28" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="82"/>
-      <c r="D28" s="83">
-        <v>0.25</v>
-      </c>
-      <c r="E28" s="84">
-        <f>F27</f>
-        <v>45908</v>
-      </c>
-      <c r="F28" s="84">
-        <f>E28+4</f>
-        <v>45912</v>
-      </c>
+      <c r="B28" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="76"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="79"/>
       <c r="G28" s="17"/>
-      <c r="H28" s="5">
+      <c r="H28" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="51"/>
-      <c r="T28" s="51"/>
-      <c r="U28" s="51"/>
-      <c r="V28" s="51"/>
-      <c r="W28" s="51"/>
-      <c r="X28" s="51"/>
-      <c r="Y28" s="51"/>
-      <c r="Z28" s="51"/>
-      <c r="AA28" s="51"/>
-      <c r="AB28" s="51"/>
-      <c r="AC28" s="51"/>
-      <c r="AD28" s="51"/>
-      <c r="AE28" s="51"/>
-      <c r="AF28" s="51"/>
-      <c r="AG28" s="51"/>
-      <c r="AH28" s="51"/>
-      <c r="AI28" s="51"/>
-      <c r="AJ28" s="51"/>
-      <c r="AK28" s="51"/>
-      <c r="AL28" s="51"/>
-      <c r="AM28" s="51"/>
-      <c r="AN28" s="51"/>
-      <c r="AO28" s="51"/>
-      <c r="AP28" s="51"/>
-      <c r="AQ28" s="51"/>
-      <c r="AR28" s="51"/>
-      <c r="AS28" s="51"/>
-      <c r="AT28" s="51"/>
-      <c r="AU28" s="51"/>
-      <c r="AV28" s="51"/>
-      <c r="AW28" s="51"/>
-      <c r="AX28" s="51"/>
-      <c r="AY28" s="51"/>
-      <c r="AZ28" s="51"/>
-      <c r="BA28" s="51"/>
-      <c r="BB28" s="51"/>
-      <c r="BC28" s="51"/>
-      <c r="BD28" s="51"/>
-      <c r="BE28" s="51"/>
-      <c r="BF28" s="51"/>
-      <c r="BG28" s="51"/>
-      <c r="BH28" s="51"/>
-      <c r="BI28" s="51"/>
-      <c r="BJ28" s="51"/>
-      <c r="BK28" s="51"/>
-      <c r="BL28" s="51"/>
+        <v/>
+      </c>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="80"/>
+      <c r="M28" s="80"/>
+      <c r="N28" s="80"/>
+      <c r="O28" s="80"/>
+      <c r="P28" s="80"/>
+      <c r="Q28" s="80"/>
+      <c r="R28" s="80"/>
+      <c r="S28" s="80"/>
+      <c r="T28" s="80"/>
+      <c r="U28" s="80"/>
+      <c r="V28" s="80"/>
+      <c r="W28" s="80"/>
+      <c r="X28" s="80"/>
+      <c r="Y28" s="80"/>
+      <c r="Z28" s="80"/>
+      <c r="AA28" s="80"/>
+      <c r="AB28" s="80"/>
+      <c r="AC28" s="80"/>
+      <c r="AD28" s="80"/>
+      <c r="AE28" s="80"/>
+      <c r="AF28" s="80"/>
+      <c r="AG28" s="80"/>
+      <c r="AH28" s="80"/>
+      <c r="AI28" s="80"/>
+      <c r="AJ28" s="80"/>
+      <c r="AK28" s="80"/>
+      <c r="AL28" s="80"/>
+      <c r="AM28" s="80"/>
+      <c r="AN28" s="80"/>
+      <c r="AO28" s="80"/>
+      <c r="AP28" s="80"/>
+      <c r="AQ28" s="80"/>
+      <c r="AR28" s="80"/>
+      <c r="AS28" s="80"/>
+      <c r="AT28" s="80"/>
+      <c r="AU28" s="80"/>
+      <c r="AV28" s="80"/>
+      <c r="AW28" s="80"/>
+      <c r="AX28" s="80"/>
+      <c r="AY28" s="80"/>
+      <c r="AZ28" s="80"/>
+      <c r="BA28" s="80"/>
+      <c r="BB28" s="80"/>
+      <c r="BC28" s="80"/>
+      <c r="BD28" s="80"/>
+      <c r="BE28" s="80"/>
+      <c r="BF28" s="80"/>
+      <c r="BG28" s="80"/>
+      <c r="BH28" s="80"/>
+      <c r="BI28" s="80"/>
+      <c r="BJ28" s="80"/>
+      <c r="BK28" s="80"/>
+      <c r="BL28" s="80"/>
     </row>
     <row r="29" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="81" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C29" s="82"/>
       <c r="D29" s="83">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E29" s="84">
-        <f>F28+1</f>
-        <v>45913</v>
+        <f>E23+2</f>
+        <v>45905</v>
       </c>
       <c r="F29" s="84">
         <f>E29+3</f>
-        <v>45916</v>
+        <v>45908</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="5">
@@ -4097,24 +4127,24 @@
     <row r="30" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="81" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C30" s="82"/>
       <c r="D30" s="83">
-        <v>0.6</v>
+        <v>0.25</v>
       </c>
       <c r="E30" s="84">
-        <f>E27+5</f>
-        <v>45910</v>
+        <f>F29</f>
+        <v>45908</v>
       </c>
       <c r="F30" s="84">
-        <f>E30+3</f>
-        <v>45913</v>
+        <f>E30+4</f>
+        <v>45912</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I30" s="51"/>
       <c r="J30" s="51"/>
@@ -4176,24 +4206,24 @@
     <row r="31" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="81" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C31" s="82"/>
       <c r="D31" s="83">
         <v>0.5</v>
       </c>
       <c r="E31" s="84">
-        <f>E27+7</f>
-        <v>45912</v>
+        <f>F30+1</f>
+        <v>45913</v>
       </c>
       <c r="F31" s="84">
-        <f>E31+5</f>
-        <v>45917</v>
+        <f>E31+3</f>
+        <v>45916</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I31" s="51"/>
       <c r="J31" s="51"/>
@@ -4254,153 +4284,311 @@
     </row>
     <row r="32" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
-      <c r="B32" s="85"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
+      <c r="B32" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="82"/>
+      <c r="D32" s="83">
+        <v>0.6</v>
+      </c>
+      <c r="E32" s="84">
+        <f>E29+5</f>
+        <v>45910</v>
+      </c>
+      <c r="F32" s="84">
+        <f>E32+3</f>
+        <v>45913</v>
+      </c>
       <c r="G32" s="17"/>
-      <c r="H32" s="5" t="str">
+      <c r="H32" s="5">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="I32" s="51"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="51"/>
+      <c r="L32" s="51"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="51"/>
+      <c r="O32" s="51"/>
+      <c r="P32" s="51"/>
+      <c r="Q32" s="51"/>
+      <c r="R32" s="51"/>
+      <c r="S32" s="51"/>
+      <c r="T32" s="51"/>
+      <c r="U32" s="51"/>
+      <c r="V32" s="51"/>
+      <c r="W32" s="51"/>
+      <c r="X32" s="51"/>
+      <c r="Y32" s="51"/>
+      <c r="Z32" s="51"/>
+      <c r="AA32" s="51"/>
+      <c r="AB32" s="51"/>
+      <c r="AC32" s="51"/>
+      <c r="AD32" s="51"/>
+      <c r="AE32" s="51"/>
+      <c r="AF32" s="51"/>
+      <c r="AG32" s="51"/>
+      <c r="AH32" s="51"/>
+      <c r="AI32" s="51"/>
+      <c r="AJ32" s="51"/>
+      <c r="AK32" s="51"/>
+      <c r="AL32" s="51"/>
+      <c r="AM32" s="51"/>
+      <c r="AN32" s="51"/>
+      <c r="AO32" s="51"/>
+      <c r="AP32" s="51"/>
+      <c r="AQ32" s="51"/>
+      <c r="AR32" s="51"/>
+      <c r="AS32" s="51"/>
+      <c r="AT32" s="51"/>
+      <c r="AU32" s="51"/>
+      <c r="AV32" s="51"/>
+      <c r="AW32" s="51"/>
+      <c r="AX32" s="51"/>
+      <c r="AY32" s="51"/>
+      <c r="AZ32" s="51"/>
+      <c r="BA32" s="51"/>
+      <c r="BB32" s="51"/>
+      <c r="BC32" s="51"/>
+      <c r="BD32" s="51"/>
+      <c r="BE32" s="51"/>
+      <c r="BF32" s="51"/>
+      <c r="BG32" s="51"/>
+      <c r="BH32" s="51"/>
+      <c r="BI32" s="51"/>
+      <c r="BJ32" s="51"/>
+      <c r="BK32" s="51"/>
+      <c r="BL32" s="51"/>
+    </row>
+    <row r="33" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
+      <c r="B33" s="81" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="82"/>
+      <c r="D33" s="83">
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="84">
+        <f>E29+7</f>
+        <v>45912</v>
+      </c>
+      <c r="F33" s="84">
+        <f>E33+5</f>
+        <v>45917</v>
+      </c>
+      <c r="G33" s="17"/>
+      <c r="H33" s="5">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="I33" s="51"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="51"/>
+      <c r="L33" s="51"/>
+      <c r="M33" s="51"/>
+      <c r="N33" s="51"/>
+      <c r="O33" s="51"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="51"/>
+      <c r="R33" s="51"/>
+      <c r="S33" s="51"/>
+      <c r="T33" s="51"/>
+      <c r="U33" s="51"/>
+      <c r="V33" s="51"/>
+      <c r="W33" s="51"/>
+      <c r="X33" s="51"/>
+      <c r="Y33" s="51"/>
+      <c r="Z33" s="51"/>
+      <c r="AA33" s="51"/>
+      <c r="AB33" s="51"/>
+      <c r="AC33" s="51"/>
+      <c r="AD33" s="51"/>
+      <c r="AE33" s="51"/>
+      <c r="AF33" s="51"/>
+      <c r="AG33" s="51"/>
+      <c r="AH33" s="51"/>
+      <c r="AI33" s="51"/>
+      <c r="AJ33" s="51"/>
+      <c r="AK33" s="51"/>
+      <c r="AL33" s="51"/>
+      <c r="AM33" s="51"/>
+      <c r="AN33" s="51"/>
+      <c r="AO33" s="51"/>
+      <c r="AP33" s="51"/>
+      <c r="AQ33" s="51"/>
+      <c r="AR33" s="51"/>
+      <c r="AS33" s="51"/>
+      <c r="AT33" s="51"/>
+      <c r="AU33" s="51"/>
+      <c r="AV33" s="51"/>
+      <c r="AW33" s="51"/>
+      <c r="AX33" s="51"/>
+      <c r="AY33" s="51"/>
+      <c r="AZ33" s="51"/>
+      <c r="BA33" s="51"/>
+      <c r="BB33" s="51"/>
+      <c r="BC33" s="51"/>
+      <c r="BD33" s="51"/>
+      <c r="BE33" s="51"/>
+      <c r="BF33" s="51"/>
+      <c r="BG33" s="51"/>
+      <c r="BH33" s="51"/>
+      <c r="BI33" s="51"/>
+      <c r="BJ33" s="51"/>
+      <c r="BK33" s="51"/>
+      <c r="BL33" s="51"/>
+    </row>
+    <row r="34" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="13"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="88"/>
+      <c r="F34" s="88"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="5" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="45"/>
-      <c r="Q32" s="45"/>
-      <c r="R32" s="45"/>
-      <c r="S32" s="45"/>
-      <c r="T32" s="45"/>
-      <c r="U32" s="45"/>
-      <c r="V32" s="45"/>
-      <c r="W32" s="45"/>
-      <c r="X32" s="45"/>
-      <c r="Y32" s="45"/>
-      <c r="Z32" s="45"/>
-      <c r="AA32" s="45"/>
-      <c r="AB32" s="45"/>
-      <c r="AC32" s="45"/>
-      <c r="AD32" s="45"/>
-      <c r="AE32" s="45"/>
-      <c r="AF32" s="45"/>
-      <c r="AG32" s="45"/>
-      <c r="AH32" s="45"/>
-      <c r="AI32" s="45"/>
-      <c r="AJ32" s="45"/>
-      <c r="AK32" s="45"/>
-      <c r="AL32" s="45"/>
-      <c r="AM32" s="45"/>
-      <c r="AN32" s="45"/>
-      <c r="AO32" s="45"/>
-      <c r="AP32" s="45"/>
-      <c r="AQ32" s="45"/>
-      <c r="AR32" s="45"/>
-      <c r="AS32" s="45"/>
-      <c r="AT32" s="45"/>
-      <c r="AU32" s="45"/>
-      <c r="AV32" s="45"/>
-      <c r="AW32" s="45"/>
-      <c r="AX32" s="45"/>
-      <c r="AY32" s="45"/>
-      <c r="AZ32" s="45"/>
-      <c r="BA32" s="45"/>
-      <c r="BB32" s="45"/>
-      <c r="BC32" s="45"/>
-      <c r="BD32" s="45"/>
-      <c r="BE32" s="45"/>
-      <c r="BF32" s="45"/>
-      <c r="BG32" s="45"/>
-      <c r="BH32" s="45"/>
-      <c r="BI32" s="45"/>
-      <c r="BJ32" s="45"/>
-      <c r="BK32" s="45"/>
-      <c r="BL32" s="45"/>
-    </row>
-    <row r="33" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
-      <c r="B33" s="89" t="s">
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="45"/>
+      <c r="T34" s="45"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="45"/>
+      <c r="W34" s="45"/>
+      <c r="X34" s="45"/>
+      <c r="Y34" s="45"/>
+      <c r="Z34" s="45"/>
+      <c r="AA34" s="45"/>
+      <c r="AB34" s="45"/>
+      <c r="AC34" s="45"/>
+      <c r="AD34" s="45"/>
+      <c r="AE34" s="45"/>
+      <c r="AF34" s="45"/>
+      <c r="AG34" s="45"/>
+      <c r="AH34" s="45"/>
+      <c r="AI34" s="45"/>
+      <c r="AJ34" s="45"/>
+      <c r="AK34" s="45"/>
+      <c r="AL34" s="45"/>
+      <c r="AM34" s="45"/>
+      <c r="AN34" s="45"/>
+      <c r="AO34" s="45"/>
+      <c r="AP34" s="45"/>
+      <c r="AQ34" s="45"/>
+      <c r="AR34" s="45"/>
+      <c r="AS34" s="45"/>
+      <c r="AT34" s="45"/>
+      <c r="AU34" s="45"/>
+      <c r="AV34" s="45"/>
+      <c r="AW34" s="45"/>
+      <c r="AX34" s="45"/>
+      <c r="AY34" s="45"/>
+      <c r="AZ34" s="45"/>
+      <c r="BA34" s="45"/>
+      <c r="BB34" s="45"/>
+      <c r="BC34" s="45"/>
+      <c r="BD34" s="45"/>
+      <c r="BE34" s="45"/>
+      <c r="BF34" s="45"/>
+      <c r="BG34" s="45"/>
+      <c r="BH34" s="45"/>
+      <c r="BI34" s="45"/>
+      <c r="BJ34" s="45"/>
+      <c r="BK34" s="45"/>
+      <c r="BL34" s="45"/>
+    </row>
+    <row r="35" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14"/>
+      <c r="B35" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="90"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="92"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="6" t="str">
+      <c r="C35" s="90"/>
+      <c r="D35" s="91"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="93"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="6" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I33" s="94"/>
-      <c r="J33" s="94"/>
-      <c r="K33" s="94"/>
-      <c r="L33" s="94"/>
-      <c r="M33" s="94"/>
-      <c r="N33" s="94"/>
-      <c r="O33" s="94"/>
-      <c r="P33" s="94"/>
-      <c r="Q33" s="94"/>
-      <c r="R33" s="94"/>
-      <c r="S33" s="94"/>
-      <c r="T33" s="94"/>
-      <c r="U33" s="94"/>
-      <c r="V33" s="94"/>
-      <c r="W33" s="94"/>
-      <c r="X33" s="94"/>
-      <c r="Y33" s="94"/>
-      <c r="Z33" s="94"/>
-      <c r="AA33" s="94"/>
-      <c r="AB33" s="94"/>
-      <c r="AC33" s="94"/>
-      <c r="AD33" s="94"/>
-      <c r="AE33" s="94"/>
-      <c r="AF33" s="94"/>
-      <c r="AG33" s="94"/>
-      <c r="AH33" s="94"/>
-      <c r="AI33" s="94"/>
-      <c r="AJ33" s="94"/>
-      <c r="AK33" s="94"/>
-      <c r="AL33" s="94"/>
-      <c r="AM33" s="94"/>
-      <c r="AN33" s="94"/>
-      <c r="AO33" s="94"/>
-      <c r="AP33" s="94"/>
-      <c r="AQ33" s="94"/>
-      <c r="AR33" s="94"/>
-      <c r="AS33" s="94"/>
-      <c r="AT33" s="94"/>
-      <c r="AU33" s="94"/>
-      <c r="AV33" s="94"/>
-      <c r="AW33" s="94"/>
-      <c r="AX33" s="94"/>
-      <c r="AY33" s="94"/>
-      <c r="AZ33" s="94"/>
-      <c r="BA33" s="94"/>
-      <c r="BB33" s="94"/>
-      <c r="BC33" s="94"/>
-      <c r="BD33" s="94"/>
-      <c r="BE33" s="94"/>
-      <c r="BF33" s="94"/>
-      <c r="BG33" s="94"/>
-      <c r="BH33" s="94"/>
-      <c r="BI33" s="94"/>
-      <c r="BJ33" s="94"/>
-      <c r="BK33" s="94"/>
-      <c r="BL33" s="94"/>
-    </row>
-    <row r="34" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="16"/>
-      <c r="F35" s="15"/>
+      <c r="I35" s="94"/>
+      <c r="J35" s="94"/>
+      <c r="K35" s="94"/>
+      <c r="L35" s="94"/>
+      <c r="M35" s="94"/>
+      <c r="N35" s="94"/>
+      <c r="O35" s="94"/>
+      <c r="P35" s="94"/>
+      <c r="Q35" s="94"/>
+      <c r="R35" s="94"/>
+      <c r="S35" s="94"/>
+      <c r="T35" s="94"/>
+      <c r="U35" s="94"/>
+      <c r="V35" s="94"/>
+      <c r="W35" s="94"/>
+      <c r="X35" s="94"/>
+      <c r="Y35" s="94"/>
+      <c r="Z35" s="94"/>
+      <c r="AA35" s="94"/>
+      <c r="AB35" s="94"/>
+      <c r="AC35" s="94"/>
+      <c r="AD35" s="94"/>
+      <c r="AE35" s="94"/>
+      <c r="AF35" s="94"/>
+      <c r="AG35" s="94"/>
+      <c r="AH35" s="94"/>
+      <c r="AI35" s="94"/>
+      <c r="AJ35" s="94"/>
+      <c r="AK35" s="94"/>
+      <c r="AL35" s="94"/>
+      <c r="AM35" s="94"/>
+      <c r="AN35" s="94"/>
+      <c r="AO35" s="94"/>
+      <c r="AP35" s="94"/>
+      <c r="AQ35" s="94"/>
+      <c r="AR35" s="94"/>
+      <c r="AS35" s="94"/>
+      <c r="AT35" s="94"/>
+      <c r="AU35" s="94"/>
+      <c r="AV35" s="94"/>
+      <c r="AW35" s="94"/>
+      <c r="AX35" s="94"/>
+      <c r="AY35" s="94"/>
+      <c r="AZ35" s="94"/>
+      <c r="BA35" s="94"/>
+      <c r="BB35" s="94"/>
+      <c r="BC35" s="94"/>
+      <c r="BD35" s="94"/>
+      <c r="BE35" s="94"/>
+      <c r="BF35" s="94"/>
+      <c r="BG35" s="94"/>
+      <c r="BH35" s="94"/>
+      <c r="BI35" s="94"/>
+      <c r="BJ35" s="94"/>
+      <c r="BK35" s="94"/>
+      <c r="BL35" s="94"/>
     </row>
     <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="4"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="16"/>
+      <c r="F37" s="15"/>
+    </row>
+    <row r="38" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -4423,7 +4611,7 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D33">
+  <conditionalFormatting sqref="D7:D35">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4437,12 +4625,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:BL31">
+  <conditionalFormatting sqref="I4:BL33">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>AND(TODAY()&gt;=I$5, TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:BL13">
+  <conditionalFormatting sqref="I9:BL15">
     <cfRule type="expression" dxfId="7" priority="6">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4450,7 +4638,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15:BL19">
+  <conditionalFormatting sqref="I17:BL21">
     <cfRule type="expression" dxfId="5" priority="4">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4458,7 +4646,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:BL25">
+  <conditionalFormatting sqref="I23:BL27">
     <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4466,7 +4654,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27:BL31">
+  <conditionalFormatting sqref="I29:BL33">
     <cfRule type="expression" dxfId="1" priority="36">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4484,12 +4672,12 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The Display week in cell Q2 is the starting week to display in the project schedule in cell I4. The project start date is Week 1. To change the display week, enter a new week number in cell Q2._x000a__x000a_Start date for each week is auto calculated starting in I4." sqref="A4" xr:uid="{43382715-6BC7-4B19-A31B-4B13A11ED166}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cells I5 through BL5 contain the day number for the week represented in the cell block above each date and are auto calculated._x000a__x000a_Today's date is outlined from today's date in row 5 through the entire date column to the end of the project schedule." sqref="A5:A6" xr:uid="{7A3789A6-A3FB-43B6-A4F7-8C0AC564F67E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B8 contains the Phase 1 sample title. Enter a new title in cell B8._x000a_To delete the phase and work only from tasks, simply delete this row." sqref="A8" xr:uid="{CEC78982-AFA8-419E-B0A2-676B709E5100}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="B9 contains the task name.  C9 is the assignee.  D9 is a progress bar that shades based on the number entered into the cell.  _x000a__x000a_E9 contains the start date and F9 contains the end date._x000a__x000a_The Gantt chart will fill in starting in cell I9 based on task dates." sqref="A9" xr:uid="{D870A2F6-6B07-4F5A-A81D-4BCCFADF8796}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A10" xr:uid="{872449A7-C3CC-45B6-BA90-B1AAD66BA0E5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A14" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A20" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A26" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A33" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="B9 contains the task name.  C9 is the assignee.  D9 is a progress bar that shades based on the number entered into the cell.  _x000a__x000a_E9 contains the start date and F9 contains the end date._x000a__x000a_The Gantt chart will fill in starting in cell I9 based on task dates." sqref="A9:A10" xr:uid="{D870A2F6-6B07-4F5A-A81D-4BCCFADF8796}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A11" xr:uid="{872449A7-C3CC-45B6-BA90-B1AAD66BA0E5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A16" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A22" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A28" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A35" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
@@ -4498,7 +4686,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F18 F22:F23 E23 F28" formula="1"/>
+    <ignoredError sqref="F20 F24:F25 E25 F30" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -4516,7 +4704,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D33</xm:sqref>
+          <xm:sqref>D7:D35</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>